<commit_message>
slimmed file only IDs no terms
</commit_message>
<xml_diff>
--- a/curator-annotations/strain-annotations/Strain_Template.xlsx
+++ b/curator-annotations/strain-annotations/Strain_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petrafey/Data/dictyBase/Overhaul/Bulk annotation files/Strain annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92B472A-5651-3A4E-B582-FF83675F2C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BF96F7-CEFD-824E-BEBD-62E2121FC110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="460" windowWidth="31400" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1720" yWindow="3220" windowWidth="31400" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strain_Annotations" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Strain Descriptor</t>
   </si>
   <si>
-    <t>Strain Names</t>
-  </si>
-  <si>
     <t>Strain Summary</t>
-  </si>
-  <si>
-    <t>Parental Strain</t>
   </si>
   <si>
     <t>Plasmid</t>
@@ -65,6 +59,12 @@
   </si>
   <si>
     <t xml:space="preserve">Systematic Name </t>
+  </si>
+  <si>
+    <t>Parental Strain ID</t>
+  </si>
+  <si>
+    <t>Strain Name(s)</t>
   </si>
 </sst>
 </file>
@@ -1278,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1290,70 +1290,66 @@
     <col min="2" max="2" width="12.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="20.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="22.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="26.1640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" style="1" customWidth="1"/>
-    <col min="15" max="17" width="10.83203125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="6" width="20.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" style="1" customWidth="1"/>
+    <col min="14" max="16" width="10.83203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1369,9 +1365,8 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1387,9 +1382,8 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1405,9 +1399,8 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1423,9 +1416,8 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1441,9 +1433,8 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1459,9 +1450,8 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1477,9 +1467,8 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1495,9 +1484,8 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1513,9 +1501,8 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1531,9 +1518,8 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1549,9 +1535,8 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-    </row>
-    <row r="13" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1567,9 +1552,8 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1585,9 +1569,8 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-    </row>
-    <row r="15" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1603,9 +1586,8 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-    </row>
-    <row r="16" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1621,9 +1603,8 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1639,9 +1620,8 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1657,9 +1637,8 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1675,9 +1654,8 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1693,9 +1671,8 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1711,9 +1688,8 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-    </row>
-    <row r="22" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1729,9 +1705,8 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-    </row>
-    <row r="23" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1747,9 +1722,8 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-    </row>
-    <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1765,9 +1739,8 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-    </row>
-    <row r="25" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1783,9 +1756,8 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-    </row>
-    <row r="26" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1801,9 +1773,8 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-    </row>
-    <row r="27" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1819,9 +1790,8 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-    </row>
-    <row r="28" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1837,9 +1807,8 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-    </row>
-    <row r="29" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1855,9 +1824,8 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-    </row>
-    <row r="30" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1873,9 +1841,8 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-    </row>
-    <row r="31" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1891,9 +1858,8 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-    </row>
-    <row r="32" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1909,9 +1875,8 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-    </row>
-    <row r="33" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1927,9 +1892,8 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-    </row>
-    <row r="34" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1945,9 +1909,8 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-    </row>
-    <row r="35" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1963,9 +1926,8 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-    </row>
-    <row r="36" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1981,9 +1943,8 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-    </row>
-    <row r="37" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1999,9 +1960,8 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-    </row>
-    <row r="38" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -2017,9 +1977,8 @@
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-    </row>
-    <row r="39" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -2035,9 +1994,8 @@
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-    </row>
-    <row r="40" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -2053,9 +2011,8 @@
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-    </row>
-    <row r="41" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -2071,9 +2028,8 @@
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-    </row>
-    <row r="42" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -2089,9 +2045,8 @@
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-    </row>
-    <row r="43" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -2107,9 +2062,8 @@
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-    </row>
-    <row r="44" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -2125,9 +2079,8 @@
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-    </row>
-    <row r="45" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -2143,9 +2096,8 @@
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-    </row>
-    <row r="46" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2161,7 +2113,6 @@
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>